<commit_message>
Working on API documentation.
</commit_message>
<xml_diff>
--- a/anystruct/excel_input_example.xlsx
+++ b/anystruct/excel_input_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ANYstructure\anystruct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A1A1FE-4254-4E0E-BA60-0BD973BB22E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F1076C-0132-48CC-8544-DA35657ECB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flate_plate" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
   <si>
     <t>Flat plate, unstiffened</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Orthogonally Stiffened panel (Stress input)</t>
-  </si>
-  <si>
-    <t>Calculation domaint</t>
   </si>
   <si>
     <t>line end 1, x</t>
@@ -229,6 +226,111 @@
   </si>
   <si>
     <t>girder type</t>
+  </si>
+  <si>
+    <t>Calculation domain</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>distance between rings</t>
+  </si>
+  <si>
+    <t>length of shell</t>
+  </si>
+  <si>
+    <t>total cyl length</t>
+  </si>
+  <si>
+    <t>buckling factor</t>
+  </si>
+  <si>
+    <t>material factor</t>
+  </si>
+  <si>
+    <t>long stf, hw</t>
+  </si>
+  <si>
+    <t>long stf, tw</t>
+  </si>
+  <si>
+    <t>long stf, bf</t>
+  </si>
+  <si>
+    <t>long stf, tf</t>
+  </si>
+  <si>
+    <t>long stf, spacing</t>
+  </si>
+  <si>
+    <t>long stf, type</t>
+  </si>
+  <si>
+    <t>ring stf, hw</t>
+  </si>
+  <si>
+    <t>ring stf, tw</t>
+  </si>
+  <si>
+    <t>ring stf, bf</t>
+  </si>
+  <si>
+    <t>ring stf, tf</t>
+  </si>
+  <si>
+    <t>girder, spacing</t>
+  </si>
+  <si>
+    <t>girder, type</t>
+  </si>
+  <si>
+    <t>stress, axial</t>
+  </si>
+  <si>
+    <t>stress, bending0</t>
+  </si>
+  <si>
+    <t>stress, torsional</t>
+  </si>
+  <si>
+    <t>stress, shear</t>
+  </si>
+  <si>
+    <t>pressure, lateral</t>
+  </si>
+  <si>
+    <t>stress, additional hoop</t>
+  </si>
+  <si>
+    <t>force, axial</t>
+  </si>
+  <si>
+    <t>force, bending</t>
+  </si>
+  <si>
+    <t>force, torsional</t>
+  </si>
+  <si>
+    <t>force, shear</t>
+  </si>
+  <si>
+    <t>limit state</t>
+  </si>
+  <si>
+    <t>material yield</t>
+  </si>
+  <si>
+    <t>ULS</t>
+  </si>
+  <si>
+    <t>FLS</t>
+  </si>
+  <si>
+    <t>line end 2, y</t>
+  </si>
+  <si>
+    <t>ring stf, type</t>
   </si>
 </sst>
 </file>
@@ -1087,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1107,76 +1209,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" t="s">
-        <v>32</v>
-      </c>
       <c r="X1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -1214,7 +1316,7 @@
         <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2">
         <v>50</v>
@@ -1270,7 +1372,7 @@
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3">
         <v>40</v>
@@ -1326,7 +1428,7 @@
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M4">
         <v>55</v>
@@ -1362,7 +1464,7 @@
         <v>20</v>
       </c>
       <c r="X4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1400,7 +1502,7 @@
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5">
         <v>98</v>
@@ -1436,7 +1538,7 @@
         <v>15</v>
       </c>
       <c r="X5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1474,7 +1576,7 @@
         <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6">
         <v>20</v>
@@ -1510,19 +1612,19 @@
         <v>20</v>
       </c>
       <c r="X6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5E31CA4-836F-49C4-B916-56D2729DAF1D}">
           <x14:formula1>
             <xm:f>Domains!$A$1:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A8</xm:sqref>
+          <xm:sqref>A7:A8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DE60D363-82B2-4FF2-913A-12E7BE0C49EB}">
           <x14:formula1>
@@ -1536,6 +1638,12 @@
           </x14:formula1>
           <xm:sqref>X2:X6</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{63150F24-5DF3-4483-82C2-328183416ED4}">
+          <x14:formula1>
+            <xm:f>Domains!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A6</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1544,22 +1652,364 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BFB5EF-D0C7-4832-9805-DD5473AFBCE9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="30" max="35" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>6000</v>
+      </c>
+      <c r="C2">
+        <v>6000</v>
+      </c>
+      <c r="D2">
+        <v>6000</v>
+      </c>
+      <c r="E2">
+        <v>15000</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5000</v>
+      </c>
+      <c r="H2">
+        <v>3300</v>
+      </c>
+      <c r="I2">
+        <v>20000</v>
+      </c>
+      <c r="J2">
+        <v>20000</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M2">
+        <v>300</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <v>150</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
+      <c r="Q2">
+        <v>700</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2">
+        <v>800</v>
+      </c>
+      <c r="Y2">
+        <v>15</v>
+      </c>
+      <c r="Z2">
+        <v>200</v>
+      </c>
+      <c r="AA2">
+        <v>20</v>
+      </c>
+      <c r="AB2">
+        <v>3300</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2">
+        <v>-100</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>-50</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>6000</v>
+      </c>
+      <c r="C3">
+        <v>15000</v>
+      </c>
+      <c r="D3">
+        <v>15000</v>
+      </c>
+      <c r="E3">
+        <v>15000</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>2000</v>
+      </c>
+      <c r="H3">
+        <v>4000</v>
+      </c>
+      <c r="I3">
+        <v>20000</v>
+      </c>
+      <c r="J3">
+        <v>20000</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M3">
+        <v>300</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>150</v>
+      </c>
+      <c r="P3">
+        <v>20</v>
+      </c>
+      <c r="Q3">
+        <v>800</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3">
+        <v>800</v>
+      </c>
+      <c r="Y3">
+        <v>15</v>
+      </c>
+      <c r="Z3">
+        <v>200</v>
+      </c>
+      <c r="AA3">
+        <v>20</v>
+      </c>
+      <c r="AB3">
+        <v>3300</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3">
+        <v>-200</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>-20</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AC53ACE-1D77-4189-AC71-49D2AC0A9357}">
+          <x14:formula1>
+            <xm:f>Domains!$A$4:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{446053ED-2064-4DC0-810A-F8EF03B51702}">
+          <x14:formula1>
+            <xm:f>Domains!$A$20:$A$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>AN2:AN3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1621,27 +2071,37 @@
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>